<commit_message>
Update work hours and last report
</commit_message>
<xml_diff>
--- a/work/RadioSens Working Hours.xlsx
+++ b/work/RadioSens Working Hours.xlsx
@@ -46,7 +46,7 @@
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="167" formatCode="d.m.yyyy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -70,6 +70,17 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="5">
@@ -145,7 +156,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
@@ -163,10 +174,10 @@
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="46" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="4" fontId="6" numFmtId="46" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -844,11 +855,11 @@
         <v>0.84375</v>
       </c>
       <c r="C32" s="12">
-        <v>0.8840277777777777</v>
+        <v>0.9020833333333333</v>
       </c>
       <c r="D32" s="4">
         <f t="shared" si="1"/>
-        <v>0.04027777778</v>
+        <v>0.05833333333</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
@@ -859,7 +870,7 @@
       </c>
       <c r="D33" s="17">
         <f>SUM(D2:D32)</f>
-        <v>4.036805556</v>
+        <v>4.054861111</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">

</xml_diff>